<commit_message>
WT assy BOM for cost report
not completed, asked PA for info
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
+++ b/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
@@ -2,29 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\WT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\Desktop\STUF2019\CR - Cost Report\BOM\WT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>System</t>
   </si>
@@ -32,20 +32,52 @@
     <t>Assembly</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Part </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(25 caractères max!)</t>
+    </r>
+  </si>
+  <si>
     <t>Make (m) / Buy (b)</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">Comments </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <charset val="1"/>
       </rPr>
       <t>(40 caractères max!)</t>
     </r>
@@ -57,154 +89,179 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Name of the part</t>
-  </si>
-  <si>
-    <t>m or b</t>
-  </si>
-  <si>
-    <t>Short description of the part</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Part </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(25 caractères max!)</t>
-    </r>
-  </si>
-  <si>
     <t>WT</t>
   </si>
   <si>
+    <t xml:space="preserve">Wheels </t>
+  </si>
+  <si>
     <t>WT_A0001</t>
   </si>
   <si>
+    <t>Oz Magnesium Rim</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>WT_01001</t>
   </si>
   <si>
+    <t>Hoosier 13"</t>
+  </si>
+  <si>
     <t>WT_01002</t>
   </si>
   <si>
-    <t>WT_01003</t>
-  </si>
-  <si>
-    <t>WT_01004</t>
-  </si>
-  <si>
-    <t>WT_01005</t>
-  </si>
-  <si>
-    <t>WT_01006</t>
+    <t>Front hubs</t>
   </si>
   <si>
     <t>WT_A0002</t>
   </si>
   <si>
+    <t>Front Hub</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
     <t>WT_02001</t>
   </si>
   <si>
+    <t>Brake Bell</t>
+  </si>
+  <si>
     <t>WT_02002</t>
   </si>
   <si>
+    <t>Front Bearing Washer</t>
+  </si>
+  <si>
     <t>WT_02003</t>
   </si>
   <si>
+    <t>Speed sensor spacer</t>
+  </si>
+  <si>
     <t>WT_02004</t>
   </si>
   <si>
+    <t>Speed sensor disc</t>
+  </si>
+  <si>
     <t>WT_02005</t>
   </si>
   <si>
+    <t>Speed sensor spacer 3mm</t>
+  </si>
+  <si>
     <t>WT_02006</t>
   </si>
   <si>
+    <t>Rear hubs</t>
+  </si>
+  <si>
     <t>WT_A0003</t>
   </si>
   <si>
+    <t>Rear Hub</t>
+  </si>
+  <si>
     <t>WT_03001</t>
   </si>
   <si>
     <t>WT_03002</t>
   </si>
   <si>
+    <t>Rear Bearing Washer</t>
+  </si>
+  <si>
     <t>WT_03003</t>
   </si>
   <si>
+    <t>Tripod Housing Spacer</t>
+  </si>
+  <si>
     <t>WT_03004</t>
   </si>
   <si>
+    <t>Speed sensor disc spacer</t>
+  </si>
+  <si>
     <t>WT_03005</t>
   </si>
   <si>
     <t>WT_03006</t>
   </si>
   <si>
-    <t xml:space="preserve">Wheels </t>
-  </si>
-  <si>
-    <t>Front hubs</t>
-  </si>
-  <si>
-    <t>Rear hubs</t>
+    <t>Speed sensor disc spacer 3mm</t>
+  </si>
+  <si>
+    <t>WT_03007</t>
+  </si>
+  <si>
+    <t>iron teeth shape like</t>
+  </si>
+  <si>
+    <t>to position WT_02004</t>
+  </si>
+  <si>
+    <t>outer side of the external bearing</t>
+  </si>
+  <si>
+    <t>rear upright vehicle inner side</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -216,20 +273,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC9DAF8"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -273,24 +330,92 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFC9DAF8"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -303,7 +428,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -348,9 +473,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -383,9 +508,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -565,26 +690,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,410 +718,336 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4">
+        <v>4</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4">
+        <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <v>2</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>2</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="F8" s="4">
+        <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>9</v>
+        <v>44</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
+        <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4">
+        <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E17" s="4" t="str">
+        <f>CONCATENATE("same as in front hub (",G9,")")</f>
+        <v>same as in front hub (WT_02004)</v>
+      </c>
+      <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="E18" s="4" t="str">
+        <f t="shared" ref="E18:E19" si="0">CONCATENATE("same as in front hub (",G10,")")</f>
+        <v>same as in front hub (WT_02005)</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>same as in front hub (WT_02006)</v>
+      </c>
+      <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WT BOM cost design report
pics and meps finalization, BOM update for speed sensor position parts
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
+++ b/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utente\Desktop\STUF2019\CR - Cost Report\BOM\WT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSAE_invictus\STUF2019\CR - Cost Report\BOM\WT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>System</t>
   </si>
@@ -203,13 +203,19 @@
     <t>iron teeth shape like</t>
   </si>
   <si>
-    <t>to position WT_02004</t>
-  </si>
-  <si>
     <t>outer side of the external bearing</t>
   </si>
   <si>
     <t>rear upright vehicle inner side</t>
+  </si>
+  <si>
+    <t>to position WT_02004 became 2mm thick</t>
+  </si>
+  <si>
+    <t>to position WT_02004 (1mm thick)</t>
+  </si>
+  <si>
+    <t>from rear brake disc deal</t>
   </si>
 </sst>
 </file>
@@ -694,7 +700,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +847,7 @@
         <v>18</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
@@ -860,9 +866,12 @@
         <v>18</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="F9" s="4">
+        <f>2*1</f>
+        <v>2</v>
+      </c>
       <c r="G9" s="4" t="s">
         <v>25</v>
       </c>
@@ -896,9 +905,12 @@
         <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="F11" s="4">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
       <c r="G11" s="4" t="s">
         <v>29</v>
       </c>
@@ -944,7 +956,9 @@
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="F14" s="4">
         <v>2</v>
       </c>
@@ -962,7 +976,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
@@ -981,7 +995,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -1003,7 +1017,10 @@
         <f>CONCATENATE("same as in front hub (",G9,")")</f>
         <v>same as in front hub (WT_02004)</v>
       </c>
-      <c r="F17" s="4"/>
+      <c r="F17" s="4">
+        <f>2*1</f>
+        <v>2</v>
+      </c>
       <c r="G17" s="4" t="s">
         <v>40</v>
       </c>
@@ -1041,7 +1058,10 @@
         <f t="shared" si="0"/>
         <v>same as in front hub (WT_02006)</v>
       </c>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
       <c r="G19" s="4" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
WT BOM cost design
ecrous, goujons, ecrous de serrage, tripod, ecrou tripod, rondelles encoche
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
+++ b/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>System</t>
   </si>
@@ -113,6 +113,18 @@
     <t>WT_01002</t>
   </si>
   <si>
+    <t>Rim Dowel</t>
+  </si>
+  <si>
+    <t>WT_01003</t>
+  </si>
+  <si>
+    <t>Rim Lock Nut</t>
+  </si>
+  <si>
+    <t>WT_01004</t>
+  </si>
+  <si>
     <t>Front hubs</t>
   </si>
   <si>
@@ -137,27 +149,66 @@
     <t>Front Bearing Washer</t>
   </si>
   <si>
+    <t>outer side of the external bearing</t>
+  </si>
+  <si>
     <t>WT_02003</t>
   </si>
   <si>
     <t>Speed sensor spacer</t>
   </si>
   <si>
+    <t>to position WT_02004 (1mm thick)</t>
+  </si>
+  <si>
     <t>WT_02004</t>
   </si>
   <si>
     <t>Speed sensor disc</t>
   </si>
   <si>
+    <t>iron teeth shape like</t>
+  </si>
+  <si>
     <t>WT_02005</t>
   </si>
   <si>
     <t>Speed sensor spacer 3mm</t>
   </si>
   <si>
+    <t>to position WT_02004 became 2mm thick</t>
+  </si>
+  <si>
     <t>WT_02006</t>
   </si>
   <si>
+    <t>Front Bearing</t>
+  </si>
+  <si>
+    <t>FAG B71910-E-2RSD-T-P4S</t>
+  </si>
+  <si>
+    <t>WT_02007</t>
+  </si>
+  <si>
+    <t>Front Hub Lock</t>
+  </si>
+  <si>
+    <t>SKF lock nut KM10</t>
+  </si>
+  <si>
+    <t>WT_02008</t>
+  </si>
+  <si>
+    <t>Front Hub Locknut Washer</t>
+  </si>
+  <si>
+    <t>SKF locknut washer MB10</t>
+  </si>
+  <si>
+    <t>WT_02009</t>
+  </si>
+  <si>
     <t>Rear hubs</t>
   </si>
   <si>
@@ -170,6 +221,9 @@
     <t>WT_03001</t>
   </si>
   <si>
+    <t>from rear brake disc deal</t>
+  </si>
+  <si>
     <t>WT_03002</t>
   </si>
   <si>
@@ -182,6 +236,9 @@
     <t>Tripod Housing Spacer</t>
   </si>
   <si>
+    <t>rear upright vehicle inner side</t>
+  </si>
+  <si>
     <t>WT_03004</t>
   </si>
   <si>
@@ -200,55 +257,22 @@
     <t>WT_03007</t>
   </si>
   <si>
-    <t>iron teeth shape like</t>
-  </si>
-  <si>
-    <t>outer side of the external bearing</t>
-  </si>
-  <si>
-    <t>rear upright vehicle inner side</t>
-  </si>
-  <si>
-    <t>to position WT_02004 became 2mm thick</t>
-  </si>
-  <si>
-    <t>to position WT_02004 (1mm thick)</t>
-  </si>
-  <si>
-    <t>from rear brake disc deal</t>
-  </si>
-  <si>
-    <t>WT_02007</t>
-  </si>
-  <si>
-    <t>goujons</t>
-  </si>
-  <si>
-    <t>ecrous</t>
-  </si>
-  <si>
-    <t>FAG B71910-E-2RSD-T-P4S</t>
-  </si>
-  <si>
-    <t>WT_02008</t>
-  </si>
-  <si>
-    <t>WT_02009</t>
-  </si>
-  <si>
-    <t>WT_02010</t>
-  </si>
-  <si>
-    <t>WT_02011</t>
-  </si>
-  <si>
-    <t>Front Bearing</t>
-  </si>
-  <si>
-    <t>Front Hub Lock Washer</t>
-  </si>
-  <si>
-    <t>Front Hub Lock</t>
+    <t xml:space="preserve">Rear Bearing </t>
+  </si>
+  <si>
+    <t>WT_03008</t>
+  </si>
+  <si>
+    <t>Tripod Housing</t>
+  </si>
+  <si>
+    <t>WT_03009</t>
+  </si>
+  <si>
+    <t>Tripod Nut</t>
+  </si>
+  <si>
+    <t>WT_03010</t>
   </si>
 </sst>
 </file>
@@ -729,11 +753,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,18 +845,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3" t="s">
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -843,45 +869,41 @@
         <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4">
-        <v>2</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="4">
         <v>2</v>
       </c>
@@ -896,237 +918,251 @@
         <v>24</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4">
-        <f>2*1</f>
         <v>2</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="F11" s="4">
-        <f>2*2</f>
-        <v>4</v>
+        <f>2*1</f>
+        <v>2</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="F12" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="4">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
       <c r="G13" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4</v>
+      </c>
       <c r="G14" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2</v>
+      </c>
       <c r="G15" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2</v>
+      </c>
       <c r="G16" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4">
         <v>2</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F21" s="4">
         <v>2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E22" s="4" t="str">
-        <f>CONCATENATE("same as in front hub (",G9,")")</f>
+        <f>CONCATENATE("same as in front hub (",G11,")")</f>
         <v>same as in front hub (WT_02004)</v>
       </c>
       <c r="F22" s="4">
@@ -1134,85 +1170,103 @@
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E23" s="4" t="str">
-        <f>CONCATENATE("same as in front hub (",G10,")")</f>
+        <f>CONCATENATE("same as in front hub (",G12,")")</f>
         <v>same as in front hub (WT_02005)</v>
       </c>
       <c r="F23" s="4">
         <v>2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E24" s="4" t="str">
-        <f>CONCATENATE("same as in front hub (",G16,")")</f>
-        <v>same as in front hub (WT_02011)</v>
+        <f>CONCATENATE("same as in front hub (",G13,")")</f>
+        <v>same as in front hub (WT_02006)</v>
       </c>
       <c r="F24" s="4">
         <f>2*2</f>
         <v>4</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="4" t="str">
+        <f>CONCATENATE("same as in front hub (",G14,")")</f>
+        <v>same as in front hub (WT_02007)</v>
+      </c>
+      <c r="F25" s="4">
+        <v>4</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="4">
+        <v>2</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="F27" s="4">
+        <v>2</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
WT BOM excel update
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
+++ b/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>System</t>
   </si>
@@ -116,15 +116,6 @@
     <t>Rim Dowel</t>
   </si>
   <si>
-    <t>WT_01003</t>
-  </si>
-  <si>
-    <t>Rim Lock Nut</t>
-  </si>
-  <si>
-    <t>WT_01004</t>
-  </si>
-  <si>
     <t>Front hubs</t>
   </si>
   <si>
@@ -158,9 +149,6 @@
     <t>Speed sensor spacer</t>
   </si>
   <si>
-    <t>to position WT_02004 (1mm thick)</t>
-  </si>
-  <si>
     <t>WT_02004</t>
   </si>
   <si>
@@ -176,18 +164,12 @@
     <t>Speed sensor spacer 3mm</t>
   </si>
   <si>
-    <t>to position WT_02004 became 2mm thick</t>
-  </si>
-  <si>
     <t>WT_02006</t>
   </si>
   <si>
     <t>Front Bearing</t>
   </si>
   <si>
-    <t>FAG B71910-E-2RSD-T-P4S</t>
-  </si>
-  <si>
     <t>WT_02007</t>
   </si>
   <si>
@@ -273,6 +255,42 @@
   </si>
   <si>
     <t>WT_03010</t>
+  </si>
+  <si>
+    <t>Rim Nut</t>
+  </si>
+  <si>
+    <t>angular contact ball bearing</t>
+  </si>
+  <si>
+    <t>to position WT_02005 (1mm thick)</t>
+  </si>
+  <si>
+    <t>to position WT_03006 (1mm thick)</t>
+  </si>
+  <si>
+    <t>to position WT_03005 became 2mm thick</t>
+  </si>
+  <si>
+    <t>hand trimmed</t>
+  </si>
+  <si>
+    <t>nylstop, non metric</t>
+  </si>
+  <si>
+    <t>to position WT_02005 became 2mm thick</t>
+  </si>
+  <si>
+    <t>WT_03011</t>
+  </si>
+  <si>
+    <t>WT_03012</t>
+  </si>
+  <si>
+    <t>WT_02010</t>
+  </si>
+  <si>
+    <t>WT_02011</t>
   </si>
 </sst>
 </file>
@@ -753,11 +771,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I15:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -828,7 +846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -845,52 +863,44 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4">
-        <v>16</v>
-      </c>
-      <c r="G6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -901,26 +911,28 @@
         <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4">
         <v>2</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="4"/>
       <c r="F9" s="4">
         <v>2</v>
       </c>
@@ -935,338 +947,407 @@
         <v>26</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4">
+        <f>2*1</f>
+        <v>2</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F10" s="4">
-        <v>2</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="4">
-        <f>2*1</f>
-        <v>2</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="4">
+        <f>2*2</f>
+        <v>4</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="4">
-        <v>2</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="F13" s="4">
-        <f>2*2</f>
         <v>4</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F14" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="F16" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
+        <v>8</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4">
-        <v>2</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="4">
-        <v>2</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>52</v>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E20" s="4"/>
       <c r="F20" s="4">
         <v>2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F21" s="4">
         <v>2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="4" t="str">
-        <f>CONCATENATE("same as in front hub (",G11,")")</f>
-        <v>same as in front hub (WT_02004)</v>
+        <v>19</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="F22" s="4">
-        <f>2*1</f>
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="4" t="str">
-        <f>CONCATENATE("same as in front hub (",G12,")")</f>
-        <v>same as in front hub (WT_02005)</v>
+        <v>19</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="F23" s="4">
         <v>2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="4" t="str">
-        <f>CONCATENATE("same as in front hub (",G13,")")</f>
-        <v>same as in front hub (WT_02006)</v>
+        <v>19</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="F24" s="4">
-        <f>2*2</f>
-        <v>4</v>
+        <f>2*1</f>
+        <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="4" t="str">
-        <f>CONCATENATE("same as in front hub (",G14,")")</f>
-        <v>same as in front hub (WT_02007)</v>
+        <v>19</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="F25" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="F26" s="4">
-        <v>2</v>
+        <f>2*2</f>
+        <v>4</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="F27" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4">
+        <v>2</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="4">
+        <v>2</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="F30" s="4">
+        <v>8</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4">
+        <v>8</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
BOM WT SU assembly
images des assemblages
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
+++ b/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\WT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSAE_invictus\STUF2019\CR - Cost Report\BOM\WT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
   <si>
     <t>System</t>
   </si>
@@ -283,11 +283,17 @@
   <si>
     <t>WT_A0200</t>
   </si>
+  <si>
+    <t>Rear Brake Disc</t>
+  </si>
+  <si>
+    <t>Front Brake Disc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,7 +422,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -500,7 +506,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -762,27 +768,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="1025" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -820,7 +826,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -837,7 +843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
@@ -854,7 +860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -869,7 +875,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -888,7 +894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
@@ -907,7 +913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
@@ -926,7 +932,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -946,7 +952,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
@@ -965,7 +971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
@@ -985,7 +991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
@@ -1004,7 +1010,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4" t="s">
@@ -1023,7 +1029,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
@@ -1042,7 +1048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
@@ -1061,7 +1067,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4" t="s">
@@ -1078,208 +1084,242 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="4">
-        <v>2</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="F21" s="4">
         <v>2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F22" s="4">
-        <f>2*1</f>
         <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="F23" s="4">
+        <f>2*1</f>
         <v>2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F24" s="4">
-        <f>2*2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F25" s="4">
+        <f>2*2</f>
         <v>4</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F26" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="F27" s="4">
         <v>8</v>
       </c>
       <c r="G27" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4">
+        <v>8</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4">
+        <v>2</v>
+      </c>
+      <c r="G29" s="4" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BOM WT brake discs
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
+++ b/CR - Cost Report/BOM/WT/WTA0100_to_WTA0300.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>System</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Front Brake Disc</t>
+  </si>
+  <si>
+    <t>WT_02012</t>
+  </si>
+  <si>
+    <t>WT_03011</t>
   </si>
 </sst>
 </file>
@@ -771,8 +777,8 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1320,7 +1326,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>